<commit_message>
Add new key and change a few things
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Cse15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="attendance" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Roll Number</t>
   </si>
@@ -23,25 +23,34 @@
     <t>Name</t>
   </si>
   <si>
-    <t>29_04_18</t>
-  </si>
-  <si>
-    <t>B17104</t>
-  </si>
-  <si>
-    <t>baba</t>
+    <t>19_05_18</t>
+  </si>
+  <si>
+    <t>24_05_18</t>
+  </si>
+  <si>
+    <t>B17085</t>
+  </si>
+  <si>
+    <t>yoy</t>
   </si>
   <si>
     <t>B17110</t>
   </si>
   <si>
-    <t>Varun</t>
-  </si>
-  <si>
-    <t>B17138</t>
-  </si>
-  <si>
-    <t>Rishi</t>
+    <t>Varun Singh</t>
+  </si>
+  <si>
+    <t>b17056</t>
+  </si>
+  <si>
+    <t>mea</t>
+  </si>
+  <si>
+    <t>b17099</t>
+  </si>
+  <si>
+    <t>me</t>
   </si>
 </sst>
 </file>
@@ -377,7 +386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,7 +394,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,33 +404,47 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3">
+    <row r="2" spans="1:4"/>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>